<commit_message>
[Abraham]:update template file excel.
</commit_message>
<xml_diff>
--- a/src/assets/anexos/creditos_preaprobados_automotriz.xlsx
+++ b/src/assets/anexos/creditos_preaprobados_automotriz.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamacone/Documents/Edgar/grp-front-center/src/assets/anexos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/papamactwo/Desktop/Project/BigPuntos/Front/grp-front-center/src/assets/anexos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A51BCBD-3BF4-244F-A168-6EDFB2A01077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A122E3F-91DA-4245-8CCF-828AFF5EA83C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="19320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,9 +118,6 @@
     <t>Mutualista Imbabura</t>
   </si>
   <si>
-    <t>1002003004001,1002003004002</t>
-  </si>
-  <si>
     <t>Saul</t>
   </si>
   <si>
@@ -143,6 +140,9 @@
   </si>
   <si>
     <t>1001807229</t>
+  </si>
+  <si>
+    <t>[1002003004001,1002003004002]</t>
   </si>
 </sst>
 </file>
@@ -1402,7 +1402,7 @@
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="14.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1509,7 +1509,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>23</v>
@@ -1518,10 +1518,10 @@
         <v>1003150602</v>
       </c>
       <c r="I2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>25</v>
@@ -1539,7 +1539,7 @@
         <v>28</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>29</v>
@@ -1554,8 +1554,8 @@
       <c r="U2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="2" t="s">
-        <v>32</v>
+      <c r="V2" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="28.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1575,16 +1575,16 @@
         <v>20</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>24</v>
@@ -1605,13 +1605,13 @@
         <v>28</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S3" s="6"/>
       <c r="T3" s="2" t="s">
@@ -1620,8 +1620,8 @@
       <c r="U3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="2" t="s">
-        <v>32</v>
+      <c r="V3" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>